<commit_message>
Add style file and update others
</commit_message>
<xml_diff>
--- a/ExperimentMatrix.xlsx
+++ b/ExperimentMatrix.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://o365coloradoedu-my.sharepoint.com/personal/cotr4663_colorado_edu/Documents/CU/Linden/Experiments/Box_Concept/Reports/SolSTAR_Phase2_DataSummary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="636" documentId="8_{5E9EE8BE-AE22-46E4-ADF7-B5FDD8B6904F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D8BF9A0-9CC1-433B-8DF1-9C09140083D7}"/>
+  <xr:revisionPtr revIDLastSave="765" documentId="8_{5E9EE8BE-AE22-46E4-ADF7-B5FDD8B6904F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B03D58D1-1865-4920-8B8B-C420DB3291CA}"/>
   <bookViews>
-    <workbookView xWindow="2892" yWindow="2892" windowWidth="17280" windowHeight="8832" firstSheet="1" activeTab="1" xr2:uid="{3FD5AFB8-BB45-44B0-A2D6-048B80984397}"/>
+    <workbookView minimized="1" xWindow="2892" yWindow="2892" windowWidth="17280" windowHeight="8832" activeTab="1" xr2:uid="{3FD5AFB8-BB45-44B0-A2D6-048B80984397}"/>
   </bookViews>
   <sheets>
     <sheet name="PotentialExperiments" sheetId="5" r:id="rId1"/>
     <sheet name="LongExperimentMatrix" sheetId="4" r:id="rId2"/>
-    <sheet name="Thermal Camera" sheetId="1" r:id="rId3"/>
-    <sheet name="Oily Soil" sheetId="2" r:id="rId4"/>
-    <sheet name="Volumes" sheetId="3" r:id="rId5"/>
+    <sheet name="Exp.MatrixSummary" sheetId="6" r:id="rId3"/>
+    <sheet name="Thermal Camera" sheetId="1" r:id="rId4"/>
+    <sheet name="Oily Soil" sheetId="2" r:id="rId5"/>
+    <sheet name="Volumes" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,8 +39,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="134">
   <si>
     <t>Variables</t>
   </si>
@@ -176,9 +199,6 @@
     <t>Date</t>
   </si>
   <si>
-    <t>Soil Type</t>
-  </si>
-  <si>
     <t>Preheat T1</t>
   </si>
   <si>
@@ -186,9 +206,6 @@
   </si>
   <si>
     <t>Peheat T3</t>
-  </si>
-  <si>
-    <t>Preheat Ave</t>
   </si>
   <si>
     <t>Ignition?</t>
@@ -295,9 +312,6 @@
     <t>Continued use after 3 Fibers</t>
   </si>
   <si>
-    <t>Yes, but not propegation</t>
-  </si>
-  <si>
     <t>Soil</t>
   </si>
   <si>
@@ -343,12 +357,6 @@
     <t>Tank Bottoms</t>
   </si>
   <si>
-    <t>~27</t>
-  </si>
-  <si>
-    <t>~63</t>
-  </si>
-  <si>
     <t>GAC Soil 50 g/kg on a 600 mL GAC bed</t>
   </si>
   <si>
@@ -400,9 +408,6 @@
     <t>Two new alumina silica gaskets</t>
   </si>
   <si>
-    <t>Max Temp</t>
-  </si>
-  <si>
     <t>Reused aerogel</t>
   </si>
   <si>
@@ -413,6 +418,94 @@
   </si>
   <si>
     <t>Same Aerogel as last experiment</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <r>
+      <t>Ave Preheat Temp (</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>°</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>C)</t>
+    </r>
+  </si>
+  <si>
+    <t>Max Temp (°C)</t>
+  </si>
+  <si>
+    <t>Yes, but not propagation</t>
   </si>
 </sst>
 </file>
@@ -423,7 +516,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -447,6 +540,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -456,7 +556,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -638,11 +738,169 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -666,6 +924,34 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1033,75 +1319,75 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C3">
         <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" t="s">
         <v>53</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>55</v>
-      </c>
-      <c r="F4" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" t="s">
         <v>55</v>
-      </c>
-      <c r="F5" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1111,1315 +1397,1432 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACB3CEA1-EF10-4579-AFBA-24E9C5CEF25C}">
-  <dimension ref="A1:X19"/>
+  <dimension ref="A1:Y19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="15" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="15" topLeftCell="D16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
-      <selection pane="bottomRight" activeCell="D18" sqref="D18"/>
+      <selection pane="bottomRight" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" customWidth="1"/>
-    <col min="8" max="8" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="12.6640625" customWidth="1"/>
-    <col min="13" max="13" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="32.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="15.109375" customWidth="1"/>
-    <col min="18" max="19" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" customWidth="1"/>
+    <col min="9" max="9" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="12.6640625" customWidth="1"/>
+    <col min="14" max="14" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="32.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="15.109375" customWidth="1"/>
+    <col min="19" max="20" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="5.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" t="s">
         <v>44</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I1" t="s">
+        <v>105</v>
+      </c>
+      <c r="J1" t="s">
+        <v>104</v>
+      </c>
+      <c r="K1" t="s">
+        <v>87</v>
+      </c>
+      <c r="L1" t="s">
+        <v>86</v>
+      </c>
+      <c r="M1" t="s">
+        <v>88</v>
+      </c>
+      <c r="N1" t="s">
+        <v>74</v>
+      </c>
+      <c r="O1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P1" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>93</v>
+      </c>
+      <c r="R1" t="s">
+        <v>94</v>
+      </c>
+      <c r="S1" t="s">
         <v>45</v>
       </c>
-      <c r="C1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="T1" t="s">
+        <v>46</v>
+      </c>
+      <c r="U1" t="s">
+        <v>47</v>
+      </c>
+      <c r="V1" t="s">
+        <v>131</v>
+      </c>
+      <c r="W1" t="s">
+        <v>132</v>
+      </c>
+      <c r="X1" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B2">
+        <v>220515</v>
+      </c>
+      <c r="C2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" t="s">
         <v>79</v>
       </c>
-      <c r="E1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F1" t="s">
-        <v>83</v>
-      </c>
-      <c r="G1" t="s">
-        <v>84</v>
-      </c>
-      <c r="H1" t="s">
-        <v>110</v>
-      </c>
-      <c r="I1" t="s">
-        <v>109</v>
-      </c>
-      <c r="J1" t="s">
-        <v>90</v>
-      </c>
-      <c r="K1" t="s">
-        <v>89</v>
-      </c>
-      <c r="L1" t="s">
-        <v>91</v>
-      </c>
-      <c r="M1" t="s">
-        <v>76</v>
-      </c>
-      <c r="N1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O1" t="s">
-        <v>72</v>
-      </c>
-      <c r="P1" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>99</v>
-      </c>
-      <c r="R1" t="s">
-        <v>46</v>
-      </c>
-      <c r="S1" t="s">
-        <v>47</v>
-      </c>
-      <c r="T1" t="s">
-        <v>48</v>
-      </c>
-      <c r="U1" t="s">
-        <v>49</v>
-      </c>
-      <c r="V1" t="s">
-        <v>113</v>
-      </c>
-      <c r="W1" t="s">
-        <v>116</v>
-      </c>
-      <c r="X1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>220515</v>
-      </c>
-      <c r="B2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E2" t="s">
-        <v>82</v>
-      </c>
-      <c r="F2">
+      <c r="G2">
         <v>20</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
-      <c r="I2" s="22">
-        <v>169.49885716860601</v>
-      </c>
-      <c r="J2" s="21">
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2" s="22">
+        <v>167.86667515193901</v>
+      </c>
+      <c r="K2" s="21">
         <v>0.67638888888888893</v>
       </c>
-      <c r="K2" s="21">
+      <c r="L2" s="21">
         <v>0.72291666666666676</v>
       </c>
-      <c r="L2" s="21">
+      <c r="M2" s="21">
         <v>0.73055555555555562</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>5</v>
       </c>
-      <c r="N2" t="s">
-        <v>52</v>
-      </c>
       <c r="O2" t="s">
-        <v>75</v>
-      </c>
-      <c r="P2">
-        <v>80</v>
+        <v>50</v>
+      </c>
+      <c r="P2" t="s">
+        <v>73</v>
       </c>
       <c r="Q2">
         <v>80</v>
       </c>
       <c r="R2">
+        <v>80</v>
+      </c>
+      <c r="S2">
         <v>207.79911972476799</v>
       </c>
-      <c r="S2">
+      <c r="T2">
         <v>231.39377272571599</v>
       </c>
-      <c r="T2">
+      <c r="U2">
         <v>184.744404312467</v>
       </c>
-      <c r="U2">
-        <f>SUM(R2:T2)/3</f>
+      <c r="V2" s="23">
+        <f>SUM(S2:U2)/3</f>
         <v>207.97909892098369</v>
       </c>
-      <c r="V2">
+      <c r="W2" s="23">
         <v>299.48306274414</v>
       </c>
-      <c r="W2">
+      <c r="X2" s="23">
         <v>67.773225499999995</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A3">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B3">
         <v>220602</v>
       </c>
-      <c r="B3" t="s">
-        <v>104</v>
-      </c>
       <c r="C3" t="s">
-        <v>68</v>
+        <v>99</v>
       </c>
       <c r="D3" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="E3" t="s">
-        <v>82</v>
-      </c>
-      <c r="F3">
+        <v>78</v>
+      </c>
+      <c r="F3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G3">
         <v>200</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>0</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>1</v>
       </c>
-      <c r="I3" s="22">
-        <v>171.159844290276</v>
-      </c>
-      <c r="J3" s="21">
+      <c r="J3" s="22">
+        <v>169.881133922233</v>
+      </c>
+      <c r="K3" s="21">
         <v>0.58888888888888891</v>
       </c>
-      <c r="K3" s="21">
+      <c r="L3" s="21">
         <v>0.6972222222222223</v>
       </c>
-      <c r="L3" s="21">
+      <c r="M3" s="21">
         <v>0.70486111111111116</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>5</v>
       </c>
-      <c r="N3" t="s">
-        <v>52</v>
-      </c>
       <c r="O3" t="s">
-        <v>75</v>
-      </c>
-      <c r="P3">
-        <v>80</v>
+        <v>50</v>
+      </c>
+      <c r="P3" t="s">
+        <v>73</v>
       </c>
       <c r="Q3">
         <v>80</v>
       </c>
       <c r="R3">
+        <v>80</v>
+      </c>
+      <c r="S3">
         <v>293.30207567826699</v>
       </c>
-      <c r="S3">
+      <c r="T3">
         <v>266.97771544109401</v>
       </c>
-      <c r="T3">
+      <c r="U3">
         <v>292.04121887753303</v>
       </c>
-      <c r="U3">
-        <f t="shared" ref="U3:U17" si="0">SUM(R3:T3)/3</f>
+      <c r="V3" s="23">
+        <f t="shared" ref="V3:V19" si="0">SUM(S3:U3)/3</f>
         <v>284.10700333229801</v>
       </c>
-      <c r="V3">
+      <c r="W3" s="23">
         <v>364.41384887695301</v>
       </c>
-      <c r="W3">
+      <c r="X3" s="23">
         <v>157.47156426666601</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A4">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B4">
         <v>220604</v>
       </c>
-      <c r="B4" t="s">
-        <v>104</v>
-      </c>
       <c r="C4" t="s">
-        <v>68</v>
+        <v>99</v>
       </c>
       <c r="D4" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="E4" t="s">
-        <v>82</v>
-      </c>
-      <c r="F4">
+        <v>78</v>
+      </c>
+      <c r="F4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G4">
         <v>200</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>0</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>2</v>
       </c>
-      <c r="I4" s="22">
-        <v>161.808151054055</v>
-      </c>
-      <c r="J4" s="21">
+      <c r="J4" s="22">
+        <v>160.422858568213</v>
+      </c>
+      <c r="K4" s="21">
         <v>0.50694444444444442</v>
       </c>
-      <c r="K4" t="s">
-        <v>55</v>
-      </c>
-      <c r="L4" s="21">
+      <c r="L4" t="s">
+        <v>53</v>
+      </c>
+      <c r="M4" s="21">
         <v>0.56597222222222221</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>5</v>
       </c>
-      <c r="N4" t="s">
-        <v>69</v>
-      </c>
       <c r="O4" t="s">
-        <v>74</v>
-      </c>
-      <c r="P4">
-        <v>0</v>
+        <v>67</v>
+      </c>
+      <c r="P4" t="s">
+        <v>72</v>
       </c>
       <c r="Q4">
         <v>0</v>
       </c>
       <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
         <v>236.74190576704299</v>
       </c>
-      <c r="S4">
+      <c r="T4">
         <v>185.46232900116601</v>
       </c>
-      <c r="T4">
+      <c r="U4">
         <v>213.11903228065</v>
       </c>
-      <c r="U4">
+      <c r="V4" s="23">
         <f t="shared" si="0"/>
         <v>211.77442234961964</v>
       </c>
-      <c r="V4">
+      <c r="W4" s="23">
         <v>336.02877807617102</v>
       </c>
-      <c r="W4">
+      <c r="X4" s="23">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A5">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B5">
         <v>220608</v>
       </c>
-      <c r="B5" t="s">
-        <v>105</v>
-      </c>
       <c r="C5" t="s">
-        <v>68</v>
+        <v>100</v>
       </c>
       <c r="D5" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="E5" t="s">
-        <v>82</v>
-      </c>
-      <c r="F5">
+        <v>78</v>
+      </c>
+      <c r="F5" t="s">
+        <v>79</v>
+      </c>
+      <c r="G5">
         <v>200</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>0</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>3</v>
       </c>
-      <c r="I5" s="22">
-        <v>178.01659602691001</v>
-      </c>
-      <c r="J5" s="21">
+      <c r="J5" s="22">
+        <v>178.19705852596999</v>
+      </c>
+      <c r="K5" s="21">
         <v>0.46666666666666662</v>
       </c>
-      <c r="K5" s="21" t="s">
-        <v>102</v>
-      </c>
-      <c r="L5" s="21">
+      <c r="L5" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="M5" s="21">
         <v>0.60763888888888895</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>5</v>
       </c>
-      <c r="N5" t="s">
-        <v>69</v>
-      </c>
       <c r="O5" t="s">
-        <v>75</v>
-      </c>
-      <c r="P5">
-        <v>80</v>
+        <v>67</v>
+      </c>
+      <c r="P5" t="s">
+        <v>73</v>
       </c>
       <c r="Q5">
         <v>80</v>
       </c>
       <c r="R5">
+        <v>80</v>
+      </c>
+      <c r="S5">
         <v>289.85779491938001</v>
       </c>
-      <c r="S5">
+      <c r="T5">
         <v>224.19043638703499</v>
       </c>
-      <c r="T5">
+      <c r="U5">
         <v>286.90306299547598</v>
       </c>
-      <c r="U5">
+      <c r="V5" s="23">
         <f t="shared" si="0"/>
         <v>266.98376476729703</v>
       </c>
-      <c r="V5">
+      <c r="W5" s="23">
         <v>404.94192504882801</v>
       </c>
-      <c r="W5">
+      <c r="X5" s="23">
         <v>109.24193305</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A6">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>117</v>
+      </c>
+      <c r="B6">
         <v>220608</v>
       </c>
-      <c r="B6" t="s">
-        <v>106</v>
-      </c>
       <c r="C6" t="s">
-        <v>68</v>
+        <v>101</v>
       </c>
       <c r="D6" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="E6" t="s">
-        <v>82</v>
-      </c>
-      <c r="F6">
+        <v>78</v>
+      </c>
+      <c r="F6" t="s">
+        <v>79</v>
+      </c>
+      <c r="G6">
         <v>200</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>0</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>4</v>
       </c>
-      <c r="I6" s="22">
-        <v>237.25741790496599</v>
-      </c>
-      <c r="J6" s="21">
+      <c r="J6" s="22">
+        <v>238.114764802439</v>
+      </c>
+      <c r="K6" s="21">
         <v>0.62638888888888888</v>
       </c>
-      <c r="K6" s="21">
+      <c r="L6" s="21">
         <v>0.67499999999999993</v>
       </c>
-      <c r="L6" s="21">
+      <c r="M6" s="21">
         <v>0.69027777777777777</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>5</v>
       </c>
-      <c r="N6" t="s">
-        <v>69</v>
-      </c>
       <c r="O6" t="s">
-        <v>73</v>
-      </c>
-      <c r="P6">
-        <v>80</v>
+        <v>67</v>
+      </c>
+      <c r="P6" t="s">
+        <v>71</v>
       </c>
       <c r="Q6">
         <v>80</v>
       </c>
       <c r="R6">
+        <v>80</v>
+      </c>
+      <c r="S6">
         <v>289.85779491938001</v>
       </c>
-      <c r="S6">
+      <c r="T6">
         <v>224.19043638703499</v>
       </c>
-      <c r="T6">
+      <c r="U6">
         <v>286.90306299547598</v>
       </c>
-      <c r="U6">
+      <c r="V6" s="23">
         <f t="shared" si="0"/>
         <v>266.98376476729703</v>
       </c>
-      <c r="V6">
+      <c r="W6" s="23">
         <v>404.94192504882801</v>
       </c>
-      <c r="W6">
+      <c r="X6" s="23">
         <v>300.24193305</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A7">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>118</v>
+      </c>
+      <c r="B7">
         <v>220610</v>
       </c>
-      <c r="B7" t="s">
-        <v>107</v>
-      </c>
       <c r="C7" t="s">
-        <v>68</v>
+        <v>102</v>
       </c>
       <c r="D7" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="E7" t="s">
-        <v>82</v>
-      </c>
-      <c r="F7">
+        <v>78</v>
+      </c>
+      <c r="F7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G7">
         <v>200</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>600</v>
       </c>
-      <c r="H7" t="s">
-        <v>88</v>
-      </c>
-      <c r="I7" s="22">
-        <v>107.54807167794699</v>
-      </c>
-      <c r="J7" s="21">
+      <c r="I7" t="s">
+        <v>85</v>
+      </c>
+      <c r="J7" s="22">
+        <v>83.168687650071206</v>
+      </c>
+      <c r="K7" s="21">
         <v>0.48194444444444445</v>
       </c>
-      <c r="K7" t="s">
-        <v>55</v>
-      </c>
-      <c r="L7" s="21">
+      <c r="L7" t="s">
+        <v>53</v>
+      </c>
+      <c r="M7" s="21">
         <v>0.57430555555555551</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <v>5</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
+        <v>69</v>
+      </c>
+      <c r="P7" t="s">
         <v>71</v>
-      </c>
-      <c r="O7" t="s">
-        <v>73</v>
-      </c>
-      <c r="P7">
-        <v>0</v>
       </c>
       <c r="Q7">
         <v>0</v>
       </c>
       <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
         <v>152.174929969418</v>
       </c>
-      <c r="S7">
+      <c r="T7">
         <v>157.11997412799099</v>
       </c>
-      <c r="T7">
+      <c r="U7">
         <v>172.78650056528099</v>
       </c>
-      <c r="U7">
+      <c r="V7" s="23">
         <f t="shared" si="0"/>
         <v>160.69380155423002</v>
       </c>
-      <c r="V7">
+      <c r="W7" s="23">
         <v>250.90249633789</v>
       </c>
-      <c r="W7">
+      <c r="X7" s="23">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A8">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>119</v>
+      </c>
+      <c r="B8">
         <v>220611</v>
       </c>
-      <c r="B8" t="s">
-        <v>107</v>
-      </c>
       <c r="C8" t="s">
-        <v>67</v>
+        <v>102</v>
       </c>
       <c r="D8" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="E8" t="s">
-        <v>82</v>
-      </c>
-      <c r="F8">
+        <v>78</v>
+      </c>
+      <c r="F8" t="s">
+        <v>79</v>
+      </c>
+      <c r="G8">
         <v>200</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>600</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>1</v>
       </c>
-      <c r="I8" s="22">
-        <v>249.487764086254</v>
-      </c>
-      <c r="J8" s="21">
+      <c r="J8" s="22">
+        <v>252.72469244550399</v>
+      </c>
+      <c r="K8" s="21">
         <v>0.45833333333333331</v>
       </c>
-      <c r="K8" s="21">
+      <c r="L8" s="21">
         <v>0.5395833333333333</v>
       </c>
-      <c r="L8" s="21">
+      <c r="M8" s="21">
         <v>0.54652777777777783</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <v>5</v>
       </c>
-      <c r="N8" t="s">
-        <v>70</v>
-      </c>
       <c r="O8" t="s">
-        <v>73</v>
-      </c>
-      <c r="P8">
-        <v>80</v>
+        <v>68</v>
+      </c>
+      <c r="P8" t="s">
+        <v>71</v>
       </c>
       <c r="Q8">
         <v>80</v>
       </c>
       <c r="R8">
+        <v>80</v>
+      </c>
+      <c r="S8">
         <v>365.706665469943</v>
       </c>
-      <c r="S8">
+      <c r="T8">
         <v>329.39724392567803</v>
       </c>
-      <c r="T8">
+      <c r="U8">
         <v>347.53649775771902</v>
       </c>
-      <c r="U8">
+      <c r="V8" s="23">
         <f t="shared" si="0"/>
         <v>347.54680238444666</v>
       </c>
-      <c r="V8">
+      <c r="W8" s="23">
         <v>790.72131347656205</v>
       </c>
-      <c r="W8">
+      <c r="X8" s="23">
         <v>123.483871299999</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A9">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>120</v>
+      </c>
+      <c r="B9">
         <v>220613</v>
       </c>
-      <c r="B9" t="s">
-        <v>85</v>
-      </c>
       <c r="C9" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="D9" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="E9" t="s">
-        <v>82</v>
-      </c>
-      <c r="F9">
+        <v>78</v>
+      </c>
+      <c r="F9" t="s">
+        <v>79</v>
+      </c>
+      <c r="G9">
         <v>200</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>600</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>0</v>
       </c>
-      <c r="I9" s="22">
-        <v>135.49808349160099</v>
-      </c>
-      <c r="J9" s="21">
+      <c r="J9" s="22">
+        <v>126.630258663934</v>
+      </c>
+      <c r="K9" s="21">
         <v>0.46666666666666662</v>
       </c>
-      <c r="K9" t="s">
-        <v>55</v>
-      </c>
-      <c r="L9" s="21">
+      <c r="L9" t="s">
+        <v>53</v>
+      </c>
+      <c r="M9" s="21">
         <v>0.48958333333333331</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>5</v>
       </c>
-      <c r="N9" t="s">
-        <v>71</v>
-      </c>
       <c r="O9" t="s">
-        <v>75</v>
-      </c>
-      <c r="R9">
+        <v>69</v>
+      </c>
+      <c r="P9" t="s">
+        <v>73</v>
+      </c>
+      <c r="S9">
         <v>323.69377550644202</v>
       </c>
-      <c r="S9">
+      <c r="T9">
         <v>294.03765577614303</v>
       </c>
-      <c r="T9">
+      <c r="U9">
         <v>345.73094927870102</v>
       </c>
-      <c r="U9">
+      <c r="V9" s="23">
         <f t="shared" si="0"/>
         <v>321.15412685376202</v>
       </c>
-      <c r="V9">
+      <c r="W9" s="23">
         <v>1021.84533691406</v>
       </c>
-      <c r="W9">
+      <c r="X9" s="23">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A10">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>121</v>
+      </c>
+      <c r="B10">
         <v>220613</v>
       </c>
-      <c r="B10" t="s">
-        <v>85</v>
-      </c>
       <c r="C10" t="s">
-        <v>67</v>
+        <v>82</v>
       </c>
       <c r="D10" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="E10" t="s">
-        <v>82</v>
-      </c>
-      <c r="F10">
+        <v>78</v>
+      </c>
+      <c r="F10" t="s">
+        <v>79</v>
+      </c>
+      <c r="G10">
         <v>200</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>600</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>1</v>
       </c>
-      <c r="I10" s="22">
-        <v>203.89814172732201</v>
-      </c>
-      <c r="J10" s="21">
+      <c r="J10" s="22">
+        <v>198.264984268338</v>
+      </c>
+      <c r="K10" s="21">
         <v>0.51597222222222217</v>
       </c>
-      <c r="K10" s="21">
+      <c r="L10" s="21">
         <v>0.61388888888888882</v>
       </c>
-      <c r="L10" s="21">
+      <c r="M10" s="21">
         <v>0.65694444444444444</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <v>5</v>
       </c>
-      <c r="N10" t="s">
-        <v>77</v>
-      </c>
       <c r="O10" t="s">
-        <v>73</v>
-      </c>
-      <c r="R10">
+        <v>75</v>
+      </c>
+      <c r="P10" t="s">
+        <v>71</v>
+      </c>
+      <c r="S10">
         <v>323.69377550644202</v>
       </c>
-      <c r="S10">
+      <c r="T10">
         <v>294.03765577614303</v>
       </c>
-      <c r="T10">
+      <c r="U10">
         <v>345.73094927870102</v>
       </c>
-      <c r="U10">
+      <c r="V10" s="23">
         <f t="shared" si="0"/>
         <v>321.15412685376202</v>
       </c>
-      <c r="V10">
+      <c r="W10" s="23">
         <v>1021.84533691406</v>
       </c>
-      <c r="W10">
+      <c r="X10" s="23">
         <v>215.55271296666601</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A11">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>122</v>
+      </c>
+      <c r="B11">
         <v>220617</v>
       </c>
-      <c r="B11" t="s">
-        <v>108</v>
-      </c>
       <c r="C11" t="s">
-        <v>67</v>
+        <v>103</v>
       </c>
       <c r="D11" t="s">
-        <v>92</v>
+        <v>65</v>
       </c>
       <c r="E11" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F11" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="G11">
+        <v>27</v>
+      </c>
+      <c r="H11">
         <v>300</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>0</v>
       </c>
-      <c r="I11" s="22">
-        <v>207.62606026945301</v>
-      </c>
-      <c r="J11" s="21">
+      <c r="J11" s="22">
+        <v>202.718220452536</v>
+      </c>
+      <c r="K11" s="21">
         <v>0.44791666666666669</v>
       </c>
-      <c r="K11" s="21">
+      <c r="L11" s="21">
         <v>0.56597222222222221</v>
       </c>
-      <c r="L11" s="21">
+      <c r="M11" s="21">
         <v>0.57430555555555551</v>
       </c>
-      <c r="M11">
+      <c r="N11">
         <v>5</v>
       </c>
-      <c r="N11" t="s">
+      <c r="O11" t="s">
+        <v>69</v>
+      </c>
+      <c r="P11" t="s">
         <v>71</v>
       </c>
-      <c r="O11" t="s">
-        <v>73</v>
-      </c>
-      <c r="R11">
+      <c r="S11">
         <v>236.28660852475801</v>
       </c>
-      <c r="S11">
+      <c r="T11">
         <v>200.62059065157899</v>
       </c>
-      <c r="T11">
+      <c r="U11">
         <v>205.06249478466401</v>
       </c>
-      <c r="U11">
+      <c r="V11" s="23">
         <f t="shared" si="0"/>
         <v>213.98989798700032</v>
       </c>
-      <c r="V11">
+      <c r="W11" s="23">
         <v>783.19421386718705</v>
       </c>
-      <c r="W11">
+      <c r="X11" s="23">
         <v>172.25021738333299</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A12">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>123</v>
+      </c>
+      <c r="B12">
         <v>220623</v>
       </c>
-      <c r="B12" t="s">
-        <v>86</v>
-      </c>
       <c r="C12" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="D12" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="E12" t="s">
-        <v>82</v>
-      </c>
-      <c r="F12">
+        <v>78</v>
+      </c>
+      <c r="F12" t="s">
+        <v>79</v>
+      </c>
+      <c r="G12">
         <v>40</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>300</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>0</v>
       </c>
-      <c r="I12" s="22">
-        <v>196.69677993837601</v>
-      </c>
-      <c r="J12" s="21">
+      <c r="J12" s="22">
+        <v>189.66249885145001</v>
+      </c>
+      <c r="K12" s="21">
         <v>0.49722222222222223</v>
       </c>
-      <c r="K12" s="21">
+      <c r="L12" s="21">
         <v>0.62152777777777779</v>
       </c>
-      <c r="L12" s="21">
+      <c r="M12" s="21">
         <v>0.68125000000000002</v>
       </c>
-      <c r="M12">
+      <c r="N12">
         <v>5</v>
       </c>
-      <c r="N12" t="s">
-        <v>114</v>
-      </c>
       <c r="O12" t="s">
-        <v>73</v>
-      </c>
-      <c r="R12">
+        <v>108</v>
+      </c>
+      <c r="P12" t="s">
+        <v>71</v>
+      </c>
+      <c r="S12">
         <v>160.66665124684701</v>
       </c>
-      <c r="S12">
+      <c r="T12">
         <v>185.07822196289899</v>
       </c>
-      <c r="T12">
+      <c r="U12">
         <v>193.30315475281401</v>
       </c>
-      <c r="U12">
+      <c r="V12" s="23">
         <f t="shared" si="0"/>
         <v>179.68267598752001</v>
       </c>
-      <c r="V12">
+      <c r="W12" s="23">
         <v>459.451080322265</v>
       </c>
-      <c r="W12">
+      <c r="X12" s="23">
         <v>218.58933528333301</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A13">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B13">
         <v>220628</v>
       </c>
-      <c r="B13" t="s">
-        <v>87</v>
-      </c>
       <c r="C13" t="s">
+        <v>84</v>
+      </c>
+      <c r="D13" t="s">
+        <v>133</v>
+      </c>
+      <c r="E13" t="s">
         <v>78</v>
       </c>
-      <c r="D13" t="s">
-        <v>81</v>
-      </c>
-      <c r="E13" t="s">
-        <v>82</v>
-      </c>
       <c r="F13" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="G13">
+        <v>63</v>
+      </c>
+      <c r="H13">
         <v>600</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>1</v>
       </c>
-      <c r="J13" s="21">
+      <c r="J13" s="22">
+        <v>228.15707039106101</v>
+      </c>
+      <c r="K13" s="21">
         <v>0.46666666666666662</v>
       </c>
-      <c r="K13" s="21">
+      <c r="L13" s="21">
         <v>0.6166666666666667</v>
       </c>
-      <c r="L13" s="21">
+      <c r="M13" s="21">
         <v>0.63194444444444442</v>
       </c>
-      <c r="M13">
+      <c r="N13">
         <v>5</v>
       </c>
-      <c r="N13" t="s">
+      <c r="O13" t="s">
+        <v>69</v>
+      </c>
+      <c r="P13" t="s">
         <v>71</v>
       </c>
-      <c r="O13" t="s">
-        <v>73</v>
-      </c>
-      <c r="R13">
+      <c r="S13">
         <v>335.30113263722598</v>
       </c>
-      <c r="S13">
+      <c r="T13">
         <v>344.49759233308401</v>
       </c>
-      <c r="T13">
+      <c r="U13">
         <v>303.22944517555902</v>
       </c>
-      <c r="U13">
+      <c r="V13" s="23">
         <f t="shared" si="0"/>
         <v>327.67605671528969</v>
       </c>
-      <c r="V13">
+      <c r="W13" s="23">
         <v>767.59033203125</v>
       </c>
-      <c r="W13">
+      <c r="X13" s="23">
         <v>222.35438793333299</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A14">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>125</v>
+      </c>
+      <c r="B14">
         <v>220708</v>
       </c>
-      <c r="B14" t="s">
-        <v>96</v>
-      </c>
       <c r="C14" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
       <c r="D14" t="s">
-        <v>97</v>
+        <v>65</v>
       </c>
       <c r="E14" t="s">
-        <v>82</v>
-      </c>
-      <c r="F14">
+        <v>92</v>
+      </c>
+      <c r="F14" t="s">
+        <v>79</v>
+      </c>
+      <c r="G14">
         <v>50</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>600</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>0</v>
       </c>
-      <c r="J14" s="21">
+      <c r="J14" s="22">
+        <v>252.98923048837401</v>
+      </c>
+      <c r="K14" s="21">
         <v>0.47083333333333338</v>
       </c>
-      <c r="K14" s="21">
+      <c r="L14" s="21">
         <v>0.58472222222222225</v>
       </c>
-      <c r="L14" s="21">
+      <c r="M14" s="21">
         <v>0.59652777777777777</v>
       </c>
-      <c r="M14">
+      <c r="N14">
         <v>5</v>
       </c>
-      <c r="N14" t="s">
+      <c r="O14" t="s">
+        <v>69</v>
+      </c>
+      <c r="P14" t="s">
         <v>71</v>
       </c>
-      <c r="O14" t="s">
-        <v>73</v>
-      </c>
-      <c r="R14">
+      <c r="S14">
         <v>282.59069218314198</v>
       </c>
-      <c r="S14">
+      <c r="T14">
         <v>266.33357379401298</v>
       </c>
-      <c r="T14">
+      <c r="U14">
         <v>307.76699464048698</v>
       </c>
-      <c r="U14">
+      <c r="V14" s="23">
         <f t="shared" si="0"/>
         <v>285.56375353921402</v>
       </c>
-      <c r="V14">
+      <c r="W14" s="23">
         <v>1369.59460449218</v>
       </c>
-      <c r="W14">
+      <c r="X14" s="23">
         <v>170.664293316666</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A15">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15">
         <v>220712</v>
       </c>
-      <c r="B15" t="s">
-        <v>100</v>
-      </c>
       <c r="C15" t="s">
-        <v>67</v>
+        <v>95</v>
       </c>
       <c r="D15" t="s">
-        <v>101</v>
+        <v>65</v>
       </c>
       <c r="E15" t="s">
-        <v>82</v>
-      </c>
-      <c r="F15">
+        <v>96</v>
+      </c>
+      <c r="F15" t="s">
+        <v>79</v>
+      </c>
+      <c r="G15">
         <v>40</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>600</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>0</v>
       </c>
-      <c r="J15" s="21">
+      <c r="J15" s="22">
+        <v>239.70233465660701</v>
+      </c>
+      <c r="K15" s="21">
         <v>0.51736111111111105</v>
       </c>
-      <c r="K15" s="21">
+      <c r="L15" s="21">
         <v>0.58333333333333337</v>
       </c>
-      <c r="L15" s="21">
+      <c r="M15" s="21">
         <v>0.59583333333333333</v>
       </c>
-      <c r="M15">
+      <c r="N15">
         <v>5</v>
       </c>
-      <c r="N15" t="s">
+      <c r="O15" t="s">
+        <v>69</v>
+      </c>
+      <c r="P15" t="s">
         <v>71</v>
       </c>
-      <c r="O15" t="s">
-        <v>73</v>
-      </c>
-      <c r="P15">
+      <c r="Q15">
         <v>50</v>
       </c>
-      <c r="Q15">
+      <c r="R15">
         <v>80</v>
       </c>
-      <c r="R15">
+      <c r="S15">
         <v>289.62135717738499</v>
       </c>
-      <c r="S15">
+      <c r="T15">
         <v>329.435792047272</v>
       </c>
-      <c r="T15">
+      <c r="U15">
         <v>314.22897860261298</v>
       </c>
-      <c r="U15">
+      <c r="V15" s="23">
         <f t="shared" si="0"/>
         <v>311.09537594242335</v>
       </c>
-      <c r="V15">
+      <c r="W15" s="23">
         <v>924.64050292968705</v>
       </c>
-      <c r="W15">
+      <c r="X15" s="23">
         <v>95.912062583333295</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A16">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>126</v>
+      </c>
+      <c r="B16">
         <v>220717</v>
       </c>
-      <c r="B16" t="s">
-        <v>111</v>
-      </c>
       <c r="C16" t="s">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="D16" t="s">
-        <v>101</v>
+        <v>65</v>
       </c>
       <c r="E16" t="s">
-        <v>82</v>
-      </c>
-      <c r="F16">
+        <v>96</v>
+      </c>
+      <c r="F16" t="s">
+        <v>79</v>
+      </c>
+      <c r="G16">
         <v>40</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>450</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>0</v>
       </c>
-      <c r="J16" s="21">
+      <c r="J16" s="22">
+        <v>248.88172298699899</v>
+      </c>
+      <c r="K16" s="21">
         <v>0.44513888888888892</v>
       </c>
-      <c r="K16" s="21">
+      <c r="L16" s="21">
         <v>0.59305555555555556</v>
       </c>
-      <c r="L16" s="21">
+      <c r="M16" s="21">
         <v>0.6069444444444444</v>
       </c>
-      <c r="M16">
+      <c r="N16">
         <v>5</v>
       </c>
-      <c r="N16" t="s">
-        <v>112</v>
-      </c>
       <c r="O16" t="s">
-        <v>73</v>
-      </c>
-      <c r="P16">
+        <v>107</v>
+      </c>
+      <c r="P16" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q16">
         <v>40</v>
       </c>
-      <c r="Q16" t="s">
-        <v>115</v>
-      </c>
-      <c r="R16">
+      <c r="R16" t="s">
+        <v>109</v>
+      </c>
+      <c r="S16">
         <v>259.04240305350299</v>
       </c>
-      <c r="S16">
+      <c r="T16">
         <v>273.67943829133799</v>
       </c>
-      <c r="T16">
+      <c r="U16">
         <v>278.484866424735</v>
       </c>
-      <c r="U16">
+      <c r="V16" s="23">
         <f t="shared" si="0"/>
         <v>270.40223592319199</v>
       </c>
-      <c r="V16">
+      <c r="W16" s="23">
         <v>631.72131347656205</v>
       </c>
-      <c r="W16">
+      <c r="X16" s="23">
         <v>214.48132254999999</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A17">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>127</v>
+      </c>
+      <c r="B17">
         <v>220719</v>
       </c>
-      <c r="B17" t="s">
-        <v>111</v>
-      </c>
       <c r="C17" t="s">
-        <v>68</v>
+        <v>106</v>
       </c>
       <c r="D17" t="s">
-        <v>101</v>
+        <v>66</v>
       </c>
       <c r="E17" t="s">
-        <v>82</v>
-      </c>
-      <c r="F17">
+        <v>96</v>
+      </c>
+      <c r="F17" t="s">
+        <v>79</v>
+      </c>
+      <c r="G17">
         <v>40</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>450</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>0</v>
       </c>
-      <c r="J17" s="21">
+      <c r="J17" s="22">
+        <v>216.930774552765</v>
+      </c>
+      <c r="K17" s="21">
         <v>0.44236111111111115</v>
       </c>
-      <c r="K17" s="21">
+      <c r="L17" s="21">
         <v>0.5229166666666667</v>
       </c>
-      <c r="L17" s="21">
+      <c r="M17" s="21">
         <v>0.52777777777777779</v>
       </c>
-      <c r="M17">
+      <c r="N17">
         <v>5</v>
       </c>
-      <c r="N17" t="s">
+      <c r="O17" t="s">
+        <v>69</v>
+      </c>
+      <c r="P17" t="s">
         <v>71</v>
       </c>
-      <c r="O17" t="s">
-        <v>73</v>
-      </c>
-      <c r="P17">
+      <c r="Q17">
         <v>30</v>
       </c>
-      <c r="Q17">
+      <c r="R17">
         <v>60</v>
       </c>
-      <c r="R17">
+      <c r="S17">
         <v>194.93626422547399</v>
       </c>
-      <c r="S17">
+      <c r="T17">
         <v>170.178327400819</v>
       </c>
-      <c r="T17">
+      <c r="U17">
         <v>186.714954723011</v>
       </c>
-      <c r="U17">
+      <c r="V17" s="23">
         <f t="shared" si="0"/>
         <v>183.94318211643466</v>
       </c>
-      <c r="V17">
+      <c r="W17" s="23">
         <v>299.04849243164</v>
       </c>
-      <c r="W17">
+      <c r="X17" s="23">
         <v>118.470813983333</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A18">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>128</v>
+      </c>
+      <c r="B18">
         <v>220720</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
+        <v>106</v>
+      </c>
+      <c r="D18" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18" t="s">
+        <v>96</v>
+      </c>
+      <c r="F18" t="s">
+        <v>79</v>
+      </c>
+      <c r="G18">
+        <v>40</v>
+      </c>
+      <c r="H18">
+        <v>450</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="J18" s="22">
+        <v>201.740493097632</v>
+      </c>
+      <c r="K18" s="21">
+        <v>0.44305555555555554</v>
+      </c>
+      <c r="L18" t="s">
+        <v>53</v>
+      </c>
+      <c r="M18" s="21">
+        <v>0.49652777777777773</v>
+      </c>
+      <c r="N18">
+        <v>5</v>
+      </c>
+      <c r="O18" t="s">
         <v>111</v>
       </c>
-      <c r="C18" t="s">
-        <v>68</v>
-      </c>
-      <c r="D18" t="s">
-        <v>101</v>
-      </c>
-      <c r="E18" t="s">
-        <v>82</v>
-      </c>
-      <c r="F18">
+      <c r="P18" t="s">
+        <v>71</v>
+      </c>
+      <c r="S18">
+        <v>196.09433618899001</v>
+      </c>
+      <c r="T18">
+        <v>221.855984146407</v>
+      </c>
+      <c r="U18">
+        <v>211.08756797859499</v>
+      </c>
+      <c r="V18" s="23">
+        <f>SUM(S18:U18)/3</f>
+        <v>209.67929610466399</v>
+      </c>
+      <c r="W18" s="23">
+        <v>285.788970947265</v>
+      </c>
+      <c r="X18" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>129</v>
+      </c>
+      <c r="B19">
+        <v>220730</v>
+      </c>
+      <c r="C19" t="s">
+        <v>106</v>
+      </c>
+      <c r="D19" t="s">
+        <v>65</v>
+      </c>
+      <c r="E19" t="s">
+        <v>96</v>
+      </c>
+      <c r="F19" t="s">
+        <v>79</v>
+      </c>
+      <c r="G19">
         <v>40</v>
       </c>
-      <c r="G18">
+      <c r="H19">
         <v>450</v>
       </c>
-      <c r="H18">
-        <v>1</v>
-      </c>
-      <c r="J18" s="21">
-        <v>0.44305555555555554</v>
-      </c>
-      <c r="K18" t="s">
-        <v>55</v>
-      </c>
-      <c r="L18" s="21">
-        <v>0.49652777777777773</v>
-      </c>
-      <c r="M18">
+      <c r="I19">
+        <v>2</v>
+      </c>
+      <c r="J19" s="22">
+        <v>247.65677179803899</v>
+      </c>
+      <c r="K19" s="21">
+        <v>0.40069444444444446</v>
+      </c>
+      <c r="L19" s="21">
+        <v>0.50486111111111109</v>
+      </c>
+      <c r="M19" s="21">
+        <v>0.52430555555555558</v>
+      </c>
+      <c r="N19">
         <v>5</v>
       </c>
-      <c r="N18" t="s">
-        <v>117</v>
-      </c>
-      <c r="O18" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>220730</v>
-      </c>
-      <c r="B19" t="s">
+      <c r="O19" t="s">
         <v>111</v>
       </c>
-      <c r="C19" t="s">
-        <v>57</v>
-      </c>
-      <c r="D19" t="s">
-        <v>101</v>
-      </c>
-      <c r="E19" t="s">
-        <v>82</v>
-      </c>
-      <c r="F19">
+      <c r="P19" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q19">
         <v>40</v>
       </c>
-      <c r="G19">
-        <v>450</v>
-      </c>
-      <c r="H19">
-        <v>2</v>
-      </c>
-      <c r="J19" s="21">
-        <v>0.40069444444444446</v>
-      </c>
-      <c r="K19" s="21">
-        <v>0.50486111111111109</v>
-      </c>
-      <c r="L19" s="21">
-        <v>0.52430555555555558</v>
-      </c>
-      <c r="M19" s="21">
-        <v>5</v>
-      </c>
-      <c r="N19" t="s">
-        <v>117</v>
-      </c>
-      <c r="O19" t="s">
-        <v>73</v>
-      </c>
-      <c r="P19">
-        <v>40</v>
-      </c>
-      <c r="Q19">
+      <c r="R19">
         <v>60</v>
       </c>
+      <c r="S19">
+        <v>278.94204091766602</v>
+      </c>
+      <c r="T19">
+        <v>286.79061614275702</v>
+      </c>
+      <c r="U19">
+        <v>283.47788164775602</v>
+      </c>
+      <c r="V19" s="23">
+        <f t="shared" si="0"/>
+        <v>283.07017956939302</v>
+      </c>
+      <c r="W19" s="23">
+        <v>739.56750488281205</v>
+      </c>
+      <c r="X19" s="23">
+        <v>155.51928393333301</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C1048576">
+  <conditionalFormatting sqref="D2:D1048576">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Yes">
-      <formula>NOT(ISERROR(SEARCH("Yes",C2)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Yes",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2428,6 +2831,766 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DFFEC7A-03DC-46EB-AFB8-1234561B43A9}">
+  <dimension ref="B1:M20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="2.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" customWidth="1"/>
+    <col min="6" max="6" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:13" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="31" t="str" cm="1">
+        <f t="array" ref="B2:B20">LongExperimentMatrix!A1:A19</f>
+        <v>ID</v>
+      </c>
+      <c r="C2" s="24" t="str" cm="1">
+        <f t="array" ref="C2:C20">LongExperimentMatrix!B1:B19</f>
+        <v>Date</v>
+      </c>
+      <c r="D2" s="31" t="str" cm="1">
+        <f t="array" ref="D2:D20">LongExperimentMatrix!C1:C19</f>
+        <v>Name</v>
+      </c>
+      <c r="E2" s="24" t="str" cm="1">
+        <f t="array" ref="E2:E20">LongExperimentMatrix!D1:D19</f>
+        <v>Ignition?</v>
+      </c>
+      <c r="F2" s="31" t="str" cm="1">
+        <f t="array" ref="F2:I20">LongExperimentMatrix!E1:H19</f>
+        <v>Soil</v>
+      </c>
+      <c r="G2" s="24" t="str">
+        <v>Contaminant</v>
+      </c>
+      <c r="H2" s="31" t="str">
+        <v>Concentration (g/kg)</v>
+      </c>
+      <c r="I2" s="24" t="str">
+        <v>GAC Bed (mL)</v>
+      </c>
+      <c r="J2" s="31" t="str" cm="1">
+        <f t="array" ref="J2:J20">LongExperimentMatrix!J1:J19</f>
+        <v>Ave. Est. Preheat Power (W)</v>
+      </c>
+      <c r="K2" s="24" t="str" cm="1">
+        <f t="array" ref="K2:M20">LongExperimentMatrix!V1:X19</f>
+        <v>Ave Preheat Temp (°C)</v>
+      </c>
+      <c r="L2" s="31" t="str">
+        <v>Max Temp (°C)</v>
+      </c>
+      <c r="M2" s="30" t="str">
+        <v>Preheat time (mins)</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B3" s="32" t="str">
+        <v>A</v>
+      </c>
+      <c r="C3" s="25">
+        <v>220515</v>
+      </c>
+      <c r="D3" s="32" t="str">
+        <v>GAC Soil 20 g/kg</v>
+      </c>
+      <c r="E3" s="25" t="str">
+        <v>No</v>
+      </c>
+      <c r="F3" s="32" t="str">
+        <v>Play Sand</v>
+      </c>
+      <c r="G3" s="25" t="str">
+        <v>GAC</v>
+      </c>
+      <c r="H3" s="32">
+        <v>20</v>
+      </c>
+      <c r="I3" s="25">
+        <v>0</v>
+      </c>
+      <c r="J3" s="35">
+        <v>167.86667515193901</v>
+      </c>
+      <c r="K3" s="28">
+        <v>207.97909892098369</v>
+      </c>
+      <c r="L3" s="35">
+        <v>299.48306274414</v>
+      </c>
+      <c r="M3" s="38">
+        <v>67.773225499999995</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B4" s="33" t="str">
+        <v>B</v>
+      </c>
+      <c r="C4" s="26">
+        <v>220602</v>
+      </c>
+      <c r="D4" s="33" t="str">
+        <v>GAC Soil 200 g/kg</v>
+      </c>
+      <c r="E4" s="26" t="str">
+        <v>No</v>
+      </c>
+      <c r="F4" s="33" t="str">
+        <v>Play Sand</v>
+      </c>
+      <c r="G4" s="26" t="str">
+        <v>GAC</v>
+      </c>
+      <c r="H4" s="33">
+        <v>200</v>
+      </c>
+      <c r="I4" s="26">
+        <v>0</v>
+      </c>
+      <c r="J4" s="36">
+        <v>169.881133922233</v>
+      </c>
+      <c r="K4" s="29">
+        <v>284.10700333229801</v>
+      </c>
+      <c r="L4" s="36">
+        <v>364.41384887695301</v>
+      </c>
+      <c r="M4" s="39">
+        <v>157.47156426666601</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B5" s="33" t="str">
+        <v>C</v>
+      </c>
+      <c r="C5" s="26">
+        <v>220604</v>
+      </c>
+      <c r="D5" s="33" t="str">
+        <v>GAC Soil 200 g/kg</v>
+      </c>
+      <c r="E5" s="26" t="str">
+        <v>No</v>
+      </c>
+      <c r="F5" s="33" t="str">
+        <v>Play Sand</v>
+      </c>
+      <c r="G5" s="26" t="str">
+        <v>GAC</v>
+      </c>
+      <c r="H5" s="33">
+        <v>200</v>
+      </c>
+      <c r="I5" s="26">
+        <v>0</v>
+      </c>
+      <c r="J5" s="36">
+        <v>160.422858568213</v>
+      </c>
+      <c r="K5" s="29">
+        <v>211.77442234961964</v>
+      </c>
+      <c r="L5" s="36">
+        <v>336.02877807617102</v>
+      </c>
+      <c r="M5" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B6" s="33" t="str">
+        <v>D</v>
+      </c>
+      <c r="C6" s="26">
+        <v>220608</v>
+      </c>
+      <c r="D6" s="33" t="str">
+        <v>GAC Soil 200 g/kg: 3 Collectors</v>
+      </c>
+      <c r="E6" s="26" t="str">
+        <v>No</v>
+      </c>
+      <c r="F6" s="33" t="str">
+        <v>Play Sand</v>
+      </c>
+      <c r="G6" s="26" t="str">
+        <v>GAC</v>
+      </c>
+      <c r="H6" s="33">
+        <v>200</v>
+      </c>
+      <c r="I6" s="26">
+        <v>0</v>
+      </c>
+      <c r="J6" s="36">
+        <v>178.19705852596999</v>
+      </c>
+      <c r="K6" s="29">
+        <v>266.98376476729703</v>
+      </c>
+      <c r="L6" s="36">
+        <v>404.94192504882801</v>
+      </c>
+      <c r="M6" s="39">
+        <v>109.24193305</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B7" s="33" t="str">
+        <v>E</v>
+      </c>
+      <c r="C7" s="26">
+        <v>220608</v>
+      </c>
+      <c r="D7" s="33" t="str">
+        <v>GAC Soil 200 g/kg: 4 Collectors</v>
+      </c>
+      <c r="E7" s="26" t="str">
+        <v>No</v>
+      </c>
+      <c r="F7" s="33" t="str">
+        <v>Play Sand</v>
+      </c>
+      <c r="G7" s="26" t="str">
+        <v>GAC</v>
+      </c>
+      <c r="H7" s="33">
+        <v>200</v>
+      </c>
+      <c r="I7" s="26">
+        <v>0</v>
+      </c>
+      <c r="J7" s="36">
+        <v>238.114764802439</v>
+      </c>
+      <c r="K7" s="29">
+        <v>266.98376476729703</v>
+      </c>
+      <c r="L7" s="36">
+        <v>404.94192504882801</v>
+      </c>
+      <c r="M7" s="39">
+        <v>300.24193305</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B8" s="33" t="str">
+        <v>F</v>
+      </c>
+      <c r="C8" s="26">
+        <v>220610</v>
+      </c>
+      <c r="D8" s="33" t="str">
+        <v>GAC Soil 200 g/kg on a 600 mL GAC bed</v>
+      </c>
+      <c r="E8" s="26" t="str">
+        <v>No</v>
+      </c>
+      <c r="F8" s="33" t="str">
+        <v>Play Sand</v>
+      </c>
+      <c r="G8" s="26" t="str">
+        <v>GAC</v>
+      </c>
+      <c r="H8" s="33">
+        <v>200</v>
+      </c>
+      <c r="I8" s="26">
+        <v>600</v>
+      </c>
+      <c r="J8" s="36">
+        <v>83.168687650071206</v>
+      </c>
+      <c r="K8" s="29">
+        <v>160.69380155423002</v>
+      </c>
+      <c r="L8" s="36">
+        <v>250.90249633789</v>
+      </c>
+      <c r="M8" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B9" s="33" t="str">
+        <v>G</v>
+      </c>
+      <c r="C9" s="26">
+        <v>220611</v>
+      </c>
+      <c r="D9" s="33" t="str">
+        <v>GAC Soil 200 g/kg on a 600 mL GAC bed</v>
+      </c>
+      <c r="E9" s="26" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="F9" s="33" t="str">
+        <v>Play Sand</v>
+      </c>
+      <c r="G9" s="26" t="str">
+        <v>GAC</v>
+      </c>
+      <c r="H9" s="33">
+        <v>200</v>
+      </c>
+      <c r="I9" s="26">
+        <v>600</v>
+      </c>
+      <c r="J9" s="36">
+        <v>252.72469244550399</v>
+      </c>
+      <c r="K9" s="29">
+        <v>347.54680238444666</v>
+      </c>
+      <c r="L9" s="36">
+        <v>790.72131347656205</v>
+      </c>
+      <c r="M9" s="39">
+        <v>123.483871299999</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B10" s="33" t="str">
+        <v>H</v>
+      </c>
+      <c r="C10" s="26">
+        <v>220613</v>
+      </c>
+      <c r="D10" s="33" t="str">
+        <v>GAC Soil 200 g/kg on a 300 mL GAC bed</v>
+      </c>
+      <c r="E10" s="26" t="str">
+        <v>No</v>
+      </c>
+      <c r="F10" s="33" t="str">
+        <v>Play Sand</v>
+      </c>
+      <c r="G10" s="26" t="str">
+        <v>GAC</v>
+      </c>
+      <c r="H10" s="33">
+        <v>200</v>
+      </c>
+      <c r="I10" s="26">
+        <v>600</v>
+      </c>
+      <c r="J10" s="36">
+        <v>126.630258663934</v>
+      </c>
+      <c r="K10" s="29">
+        <v>321.15412685376202</v>
+      </c>
+      <c r="L10" s="36">
+        <v>1021.84533691406</v>
+      </c>
+      <c r="M10" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B11" s="33" t="str">
+        <v>I</v>
+      </c>
+      <c r="C11" s="26">
+        <v>220613</v>
+      </c>
+      <c r="D11" s="33" t="str">
+        <v>GAC Soil 200 g/kg on a 300 mL GAC bed</v>
+      </c>
+      <c r="E11" s="26" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="F11" s="33" t="str">
+        <v>Play Sand</v>
+      </c>
+      <c r="G11" s="26" t="str">
+        <v>GAC</v>
+      </c>
+      <c r="H11" s="33">
+        <v>200</v>
+      </c>
+      <c r="I11" s="26">
+        <v>600</v>
+      </c>
+      <c r="J11" s="36">
+        <v>198.264984268338</v>
+      </c>
+      <c r="K11" s="29">
+        <v>321.15412685376202</v>
+      </c>
+      <c r="L11" s="36">
+        <v>1021.84533691406</v>
+      </c>
+      <c r="M11" s="39">
+        <v>215.55271296666601</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B12" s="33" t="str">
+        <v>J</v>
+      </c>
+      <c r="C12" s="26">
+        <v>220617</v>
+      </c>
+      <c r="D12" s="33" t="str">
+        <v>Road Mix on a 300 mL GAC bed</v>
+      </c>
+      <c r="E12" s="26" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="F12" s="33" t="str">
+        <v>Local Soil</v>
+      </c>
+      <c r="G12" s="26" t="str">
+        <v>Tank Bottoms</v>
+      </c>
+      <c r="H12" s="33">
+        <v>27</v>
+      </c>
+      <c r="I12" s="26">
+        <v>300</v>
+      </c>
+      <c r="J12" s="36">
+        <v>202.718220452536</v>
+      </c>
+      <c r="K12" s="29">
+        <v>213.98989798700032</v>
+      </c>
+      <c r="L12" s="36">
+        <v>783.19421386718705</v>
+      </c>
+      <c r="M12" s="39">
+        <v>172.25021738333299</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B13" s="33" t="str">
+        <v>K</v>
+      </c>
+      <c r="C13" s="26">
+        <v>220623</v>
+      </c>
+      <c r="D13" s="33" t="str">
+        <v>GAC Soil 40 g/kg on a 300 mL GAC bed</v>
+      </c>
+      <c r="E13" s="26" t="str">
+        <v>No</v>
+      </c>
+      <c r="F13" s="33" t="str">
+        <v>Play Sand</v>
+      </c>
+      <c r="G13" s="26" t="str">
+        <v>GAC</v>
+      </c>
+      <c r="H13" s="33">
+        <v>40</v>
+      </c>
+      <c r="I13" s="26">
+        <v>300</v>
+      </c>
+      <c r="J13" s="36">
+        <v>189.66249885145001</v>
+      </c>
+      <c r="K13" s="29">
+        <v>179.68267598752001</v>
+      </c>
+      <c r="L13" s="36">
+        <v>459.451080322265</v>
+      </c>
+      <c r="M13" s="39">
+        <v>218.58933528333301</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B14" s="33" t="str">
+        <v>L</v>
+      </c>
+      <c r="C14" s="26">
+        <v>220628</v>
+      </c>
+      <c r="D14" s="33" t="str">
+        <v>GAC Soil 60 g/kg on a 600 mL GAC bed</v>
+      </c>
+      <c r="E14" s="27" t="str">
+        <v>Yes, but not propagation</v>
+      </c>
+      <c r="F14" s="33" t="str">
+        <v>Play Sand</v>
+      </c>
+      <c r="G14" s="26" t="str">
+        <v>GAC</v>
+      </c>
+      <c r="H14" s="33">
+        <v>63</v>
+      </c>
+      <c r="I14" s="26">
+        <v>600</v>
+      </c>
+      <c r="J14" s="36">
+        <v>228.15707039106101</v>
+      </c>
+      <c r="K14" s="29">
+        <v>327.67605671528969</v>
+      </c>
+      <c r="L14" s="36">
+        <v>767.59033203125</v>
+      </c>
+      <c r="M14" s="39">
+        <v>222.35438793333299</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B15" s="33" t="str">
+        <v>M</v>
+      </c>
+      <c r="C15" s="26">
+        <v>220708</v>
+      </c>
+      <c r="D15" s="33" t="str">
+        <v>GAC Soil 50 g/kg on a 600 mL GAC bed</v>
+      </c>
+      <c r="E15" s="26" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="F15" s="33" t="str">
+        <v>Aquarium Sand</v>
+      </c>
+      <c r="G15" s="26" t="str">
+        <v>GAC</v>
+      </c>
+      <c r="H15" s="33">
+        <v>50</v>
+      </c>
+      <c r="I15" s="26">
+        <v>600</v>
+      </c>
+      <c r="J15" s="36">
+        <v>252.98923048837401</v>
+      </c>
+      <c r="K15" s="29">
+        <v>285.56375353921402</v>
+      </c>
+      <c r="L15" s="36">
+        <v>1369.59460449218</v>
+      </c>
+      <c r="M15" s="39">
+        <v>170.664293316666</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B16" s="33" t="str">
+        <v>N</v>
+      </c>
+      <c r="C16" s="26">
+        <v>220712</v>
+      </c>
+      <c r="D16" s="33" t="str">
+        <v>GAC Soil 40 g/kg on a 600 mL GAC bed</v>
+      </c>
+      <c r="E16" s="26" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="F16" s="33" t="str">
+        <v>Pool Sand</v>
+      </c>
+      <c r="G16" s="26" t="str">
+        <v>GAC</v>
+      </c>
+      <c r="H16" s="33">
+        <v>40</v>
+      </c>
+      <c r="I16" s="26">
+        <v>600</v>
+      </c>
+      <c r="J16" s="36">
+        <v>239.70233465660701</v>
+      </c>
+      <c r="K16" s="29">
+        <v>311.09537594242335</v>
+      </c>
+      <c r="L16" s="36">
+        <v>924.64050292968705</v>
+      </c>
+      <c r="M16" s="39">
+        <v>95.912062583333295</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B17" s="33" t="str">
+        <v>O</v>
+      </c>
+      <c r="C17" s="26">
+        <v>220717</v>
+      </c>
+      <c r="D17" s="33" t="str">
+        <v>GAC Soil 40 g/kg on a 450 mL GAC bed</v>
+      </c>
+      <c r="E17" s="26" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="F17" s="33" t="str">
+        <v>Pool Sand</v>
+      </c>
+      <c r="G17" s="26" t="str">
+        <v>GAC</v>
+      </c>
+      <c r="H17" s="33">
+        <v>40</v>
+      </c>
+      <c r="I17" s="26">
+        <v>450</v>
+      </c>
+      <c r="J17" s="36">
+        <v>248.88172298699899</v>
+      </c>
+      <c r="K17" s="29">
+        <v>270.40223592319199</v>
+      </c>
+      <c r="L17" s="36">
+        <v>631.72131347656205</v>
+      </c>
+      <c r="M17" s="39">
+        <v>214.48132254999999</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B18" s="33" t="str">
+        <v>P</v>
+      </c>
+      <c r="C18" s="26">
+        <v>220719</v>
+      </c>
+      <c r="D18" s="33" t="str">
+        <v>GAC Soil 40 g/kg on a 450 mL GAC bed</v>
+      </c>
+      <c r="E18" s="26" t="str">
+        <v>No</v>
+      </c>
+      <c r="F18" s="33" t="str">
+        <v>Pool Sand</v>
+      </c>
+      <c r="G18" s="26" t="str">
+        <v>GAC</v>
+      </c>
+      <c r="H18" s="33">
+        <v>40</v>
+      </c>
+      <c r="I18" s="26">
+        <v>450</v>
+      </c>
+      <c r="J18" s="36">
+        <v>216.930774552765</v>
+      </c>
+      <c r="K18" s="29">
+        <v>183.94318211643466</v>
+      </c>
+      <c r="L18" s="36">
+        <v>299.04849243164</v>
+      </c>
+      <c r="M18" s="39">
+        <v>118.470813983333</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B19" s="33" t="str">
+        <v>Q</v>
+      </c>
+      <c r="C19" s="26">
+        <v>220720</v>
+      </c>
+      <c r="D19" s="33" t="str">
+        <v>GAC Soil 40 g/kg on a 450 mL GAC bed</v>
+      </c>
+      <c r="E19" s="26" t="str">
+        <v>No</v>
+      </c>
+      <c r="F19" s="33" t="str">
+        <v>Pool Sand</v>
+      </c>
+      <c r="G19" s="26" t="str">
+        <v>GAC</v>
+      </c>
+      <c r="H19" s="33">
+        <v>40</v>
+      </c>
+      <c r="I19" s="26">
+        <v>450</v>
+      </c>
+      <c r="J19" s="36">
+        <v>201.740493097632</v>
+      </c>
+      <c r="K19" s="29">
+        <v>209.67929610466399</v>
+      </c>
+      <c r="L19" s="36">
+        <v>285.788970947265</v>
+      </c>
+      <c r="M19" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="34" t="str">
+        <v>R</v>
+      </c>
+      <c r="C20" s="40">
+        <v>220730</v>
+      </c>
+      <c r="D20" s="34" t="str">
+        <v>GAC Soil 40 g/kg on a 450 mL GAC bed</v>
+      </c>
+      <c r="E20" s="40" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="F20" s="34" t="str">
+        <v>Pool Sand</v>
+      </c>
+      <c r="G20" s="40" t="str">
+        <v>GAC</v>
+      </c>
+      <c r="H20" s="34">
+        <v>40</v>
+      </c>
+      <c r="I20" s="40">
+        <v>450</v>
+      </c>
+      <c r="J20" s="37">
+        <v>247.65677179803899</v>
+      </c>
+      <c r="K20" s="41">
+        <v>283.07017956939302</v>
+      </c>
+      <c r="L20" s="37">
+        <v>739.56750488281205</v>
+      </c>
+      <c r="M20" s="42">
+        <v>155.51928393333301</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9027072-2CB2-4AD0-9DB0-73716D6F3E27}">
   <dimension ref="A1:K6"/>
   <sheetViews>
@@ -2552,7 +3715,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{563F98B6-A947-4FC1-AB0D-253E5323B3BE}">
   <dimension ref="A1:D6"/>
   <sheetViews>
@@ -2632,7 +3795,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DED17B8-4286-4B63-81EB-11E86383FBEB}">
   <dimension ref="A1:H10"/>
   <sheetViews>

</xml_diff>